<commit_message>
A1 FIS en Dobles Grados
</commit_message>
<xml_diff>
--- a/jesus/Horarios GIIADE (24-25).xlsx
+++ b/jesus/Horarios GIIADE (24-25).xlsx
@@ -1808,7 +1808,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="266">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2554,10 +2554,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2957,7 +2953,7 @@
   </sheetPr>
   <dimension ref="A2:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L46" activeCellId="0" sqref="L46"/>
     </sheetView>
   </sheetViews>
@@ -4395,8 +4391,8 @@
     <mergeCell ref="A58:A59"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="40" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="40" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4409,10 +4405,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:P1048576"/>
+  <dimension ref="A2:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F28" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O48" activeCellId="0" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5294,20 +5290,19 @@
       <c r="M46" s="168"/>
       <c r="N46" s="186"/>
       <c r="O46" s="186"/>
-      <c r="P46" s="187"/>
     </row>
     <row r="47" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="188"/>
-      <c r="B47" s="188"/>
-      <c r="C47" s="188"/>
-      <c r="D47" s="188"/>
-      <c r="E47" s="188"/>
-      <c r="F47" s="188"/>
-      <c r="G47" s="188"/>
-      <c r="H47" s="188"/>
-      <c r="I47" s="188"/>
-      <c r="J47" s="188"/>
-      <c r="K47" s="188"/>
+      <c r="A47" s="187"/>
+      <c r="B47" s="187"/>
+      <c r="C47" s="187"/>
+      <c r="D47" s="187"/>
+      <c r="E47" s="187"/>
+      <c r="F47" s="187"/>
+      <c r="G47" s="187"/>
+      <c r="H47" s="187"/>
+      <c r="I47" s="187"/>
+      <c r="J47" s="187"/>
+      <c r="K47" s="187"/>
       <c r="L47" s="167"/>
       <c r="M47" s="168"/>
       <c r="N47" s="167"/>
@@ -5316,32 +5311,32 @@
       <c r="A48" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="189"/>
+      <c r="B48" s="188"/>
       <c r="C48" s="136"/>
       <c r="D48" s="135"/>
       <c r="E48" s="136"/>
-      <c r="F48" s="189"/>
+      <c r="F48" s="188"/>
       <c r="G48" s="136"/>
       <c r="H48" s="135"/>
       <c r="I48" s="136"/>
       <c r="J48" s="135"/>
-      <c r="K48" s="190"/>
+      <c r="K48" s="189"/>
       <c r="L48" s="167"/>
       <c r="M48" s="168"/>
       <c r="N48" s="167"/>
     </row>
     <row r="49" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="58"/>
-      <c r="B49" s="191"/>
+      <c r="B49" s="190"/>
       <c r="C49" s="139"/>
       <c r="D49" s="138"/>
       <c r="E49" s="139"/>
-      <c r="F49" s="191"/>
+      <c r="F49" s="190"/>
       <c r="G49" s="139"/>
       <c r="H49" s="138"/>
       <c r="I49" s="139"/>
       <c r="J49" s="138"/>
-      <c r="K49" s="192"/>
+      <c r="K49" s="191"/>
     </row>
     <row r="50" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="67" t="s">
@@ -5361,14 +5356,14 @@
     <row r="51" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="67"/>
       <c r="B51" s="184"/>
-      <c r="C51" s="193"/>
-      <c r="D51" s="194"/>
-      <c r="E51" s="193"/>
-      <c r="F51" s="194"/>
-      <c r="G51" s="193"/>
-      <c r="H51" s="194"/>
-      <c r="I51" s="193"/>
-      <c r="J51" s="194"/>
+      <c r="C51" s="192"/>
+      <c r="D51" s="193"/>
+      <c r="E51" s="192"/>
+      <c r="F51" s="193"/>
+      <c r="G51" s="192"/>
+      <c r="H51" s="193"/>
+      <c r="I51" s="192"/>
+      <c r="J51" s="193"/>
       <c r="K51" s="185"/>
     </row>
     <row r="52" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5388,7 +5383,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="67"/>
-      <c r="B53" s="195"/>
+      <c r="B53" s="194"/>
       <c r="C53" s="127"/>
       <c r="D53" s="146"/>
       <c r="E53" s="127"/>
@@ -5397,7 +5392,7 @@
       <c r="H53" s="146"/>
       <c r="I53" s="127"/>
       <c r="J53" s="146"/>
-      <c r="K53" s="196"/>
+      <c r="K53" s="195"/>
     </row>
     <row r="54" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="67" t="s">
@@ -5416,7 +5411,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="67"/>
-      <c r="B55" s="195"/>
+      <c r="B55" s="194"/>
       <c r="C55" s="131"/>
       <c r="D55" s="146"/>
       <c r="E55" s="131"/>
@@ -5425,7 +5420,7 @@
       <c r="H55" s="146"/>
       <c r="I55" s="131"/>
       <c r="J55" s="146"/>
-      <c r="K55" s="197"/>
+      <c r="K55" s="196"/>
     </row>
     <row r="56" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="67" t="s">
@@ -5444,7 +5439,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="67"/>
-      <c r="B57" s="195"/>
+      <c r="B57" s="194"/>
       <c r="C57" s="127"/>
       <c r="D57" s="146"/>
       <c r="E57" s="127"/>
@@ -5453,35 +5448,35 @@
       <c r="H57" s="146"/>
       <c r="I57" s="127"/>
       <c r="J57" s="146"/>
-      <c r="K57" s="196"/>
+      <c r="K57" s="195"/>
     </row>
     <row r="58" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="B58" s="198"/>
-      <c r="C58" s="198"/>
-      <c r="D58" s="199"/>
-      <c r="E58" s="199"/>
-      <c r="F58" s="198"/>
-      <c r="G58" s="198"/>
-      <c r="H58" s="199"/>
-      <c r="I58" s="199"/>
-      <c r="J58" s="200"/>
-      <c r="K58" s="200"/>
+      <c r="B58" s="197"/>
+      <c r="C58" s="197"/>
+      <c r="D58" s="198"/>
+      <c r="E58" s="198"/>
+      <c r="F58" s="197"/>
+      <c r="G58" s="197"/>
+      <c r="H58" s="198"/>
+      <c r="I58" s="198"/>
+      <c r="J58" s="199"/>
+      <c r="K58" s="199"/>
     </row>
     <row r="59" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="74"/>
-      <c r="B59" s="201"/>
-      <c r="C59" s="202"/>
-      <c r="D59" s="203"/>
-      <c r="E59" s="202"/>
-      <c r="F59" s="201"/>
-      <c r="G59" s="202"/>
-      <c r="H59" s="203"/>
-      <c r="I59" s="202"/>
-      <c r="J59" s="203"/>
-      <c r="K59" s="204"/>
+      <c r="B59" s="200"/>
+      <c r="C59" s="201"/>
+      <c r="D59" s="202"/>
+      <c r="E59" s="201"/>
+      <c r="F59" s="200"/>
+      <c r="G59" s="201"/>
+      <c r="H59" s="202"/>
+      <c r="I59" s="201"/>
+      <c r="J59" s="202"/>
+      <c r="K59" s="203"/>
     </row>
     <row r="1048438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5716,8 +5711,8 @@
     <mergeCell ref="J58:K58"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="55" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="55" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5732,7 +5727,7 @@
   </sheetPr>
   <dimension ref="A2:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C31" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J55" activeCellId="0" sqref="J55"/>
     </sheetView>
   </sheetViews>
@@ -5811,71 +5806,71 @@
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="205"/>
-      <c r="C5" s="205"/>
-      <c r="D5" s="205"/>
-      <c r="E5" s="205"/>
-      <c r="F5" s="205"/>
-      <c r="G5" s="205"/>
-      <c r="H5" s="205"/>
-      <c r="I5" s="205"/>
-      <c r="J5" s="205"/>
-      <c r="K5" s="205"/>
-      <c r="L5" s="205"/>
-      <c r="M5" s="205"/>
-      <c r="N5" s="205"/>
+      <c r="B5" s="204"/>
+      <c r="C5" s="204"/>
+      <c r="D5" s="204"/>
+      <c r="E5" s="204"/>
+      <c r="F5" s="204"/>
+      <c r="G5" s="204"/>
+      <c r="H5" s="204"/>
+      <c r="I5" s="204"/>
+      <c r="J5" s="204"/>
+      <c r="K5" s="204"/>
+      <c r="L5" s="204"/>
+      <c r="M5" s="204"/>
+      <c r="N5" s="204"/>
     </row>
     <row r="6" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
-      <c r="B6" s="206"/>
-      <c r="C6" s="206"/>
-      <c r="D6" s="206"/>
-      <c r="E6" s="206"/>
-      <c r="F6" s="206"/>
-      <c r="G6" s="206"/>
-      <c r="H6" s="206"/>
-      <c r="I6" s="206"/>
-      <c r="J6" s="206"/>
-      <c r="K6" s="206"/>
-      <c r="L6" s="206"/>
-      <c r="M6" s="206"/>
-      <c r="N6" s="206"/>
+      <c r="B6" s="205"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="205"/>
+      <c r="E6" s="205"/>
+      <c r="F6" s="205"/>
+      <c r="G6" s="205"/>
+      <c r="H6" s="205"/>
+      <c r="I6" s="205"/>
+      <c r="J6" s="205"/>
+      <c r="K6" s="205"/>
+      <c r="L6" s="205"/>
+      <c r="M6" s="205"/>
+      <c r="N6" s="205"/>
     </row>
     <row r="7" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="199"/>
-      <c r="C7" s="199"/>
-      <c r="D7" s="199"/>
-      <c r="E7" s="199"/>
-      <c r="F7" s="199"/>
-      <c r="G7" s="199"/>
-      <c r="H7" s="199"/>
-      <c r="I7" s="199"/>
-      <c r="J7" s="199"/>
-      <c r="K7" s="199"/>
-      <c r="L7" s="199"/>
-      <c r="M7" s="199"/>
-      <c r="N7" s="199"/>
+      <c r="B7" s="198"/>
+      <c r="C7" s="198"/>
+      <c r="D7" s="198"/>
+      <c r="E7" s="198"/>
+      <c r="F7" s="198"/>
+      <c r="G7" s="198"/>
+      <c r="H7" s="198"/>
+      <c r="I7" s="198"/>
+      <c r="J7" s="198"/>
+      <c r="K7" s="198"/>
+      <c r="L7" s="198"/>
+      <c r="M7" s="198"/>
+      <c r="N7" s="198"/>
       <c r="O7" s="34"/>
       <c r="P7" s="35"/>
     </row>
     <row r="8" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="24"/>
-      <c r="B8" s="206"/>
-      <c r="C8" s="206"/>
-      <c r="D8" s="206"/>
-      <c r="E8" s="206"/>
-      <c r="F8" s="206"/>
-      <c r="G8" s="206"/>
-      <c r="H8" s="206"/>
-      <c r="I8" s="206"/>
-      <c r="J8" s="206"/>
-      <c r="K8" s="206"/>
-      <c r="L8" s="206"/>
-      <c r="M8" s="206"/>
-      <c r="N8" s="206"/>
+      <c r="B8" s="205"/>
+      <c r="C8" s="205"/>
+      <c r="D8" s="205"/>
+      <c r="E8" s="205"/>
+      <c r="F8" s="205"/>
+      <c r="G8" s="205"/>
+      <c r="H8" s="205"/>
+      <c r="I8" s="205"/>
+      <c r="J8" s="205"/>
+      <c r="K8" s="205"/>
+      <c r="L8" s="205"/>
+      <c r="M8" s="205"/>
+      <c r="N8" s="205"/>
       <c r="O8" s="36"/>
       <c r="P8" s="36"/>
     </row>
@@ -5883,37 +5878,37 @@
       <c r="A9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="199"/>
-      <c r="C9" s="199"/>
-      <c r="D9" s="199"/>
-      <c r="E9" s="199"/>
-      <c r="F9" s="199"/>
-      <c r="G9" s="199"/>
-      <c r="H9" s="199"/>
-      <c r="I9" s="199"/>
-      <c r="J9" s="199"/>
-      <c r="K9" s="199"/>
-      <c r="L9" s="199"/>
-      <c r="M9" s="199"/>
-      <c r="N9" s="199"/>
+      <c r="B9" s="198"/>
+      <c r="C9" s="198"/>
+      <c r="D9" s="198"/>
+      <c r="E9" s="198"/>
+      <c r="F9" s="198"/>
+      <c r="G9" s="198"/>
+      <c r="H9" s="198"/>
+      <c r="I9" s="198"/>
+      <c r="J9" s="198"/>
+      <c r="K9" s="198"/>
+      <c r="L9" s="198"/>
+      <c r="M9" s="198"/>
+      <c r="N9" s="198"/>
       <c r="O9" s="36"/>
       <c r="P9" s="70"/>
     </row>
     <row r="10" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="24"/>
-      <c r="B10" s="206"/>
-      <c r="C10" s="206"/>
-      <c r="D10" s="206"/>
-      <c r="E10" s="206"/>
-      <c r="F10" s="206"/>
-      <c r="G10" s="206"/>
-      <c r="H10" s="206"/>
-      <c r="I10" s="206"/>
-      <c r="J10" s="206"/>
-      <c r="K10" s="206"/>
-      <c r="L10" s="206"/>
-      <c r="M10" s="206"/>
-      <c r="N10" s="206"/>
+      <c r="B10" s="205"/>
+      <c r="C10" s="205"/>
+      <c r="D10" s="205"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="205"/>
+      <c r="G10" s="205"/>
+      <c r="H10" s="205"/>
+      <c r="I10" s="205"/>
+      <c r="J10" s="205"/>
+      <c r="K10" s="205"/>
+      <c r="L10" s="205"/>
+      <c r="M10" s="205"/>
+      <c r="N10" s="205"/>
       <c r="O10" s="36"/>
       <c r="P10" s="36"/>
     </row>
@@ -5921,37 +5916,37 @@
       <c r="A11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="199"/>
-      <c r="C11" s="199"/>
-      <c r="D11" s="199"/>
-      <c r="E11" s="199"/>
-      <c r="F11" s="199"/>
-      <c r="G11" s="199"/>
-      <c r="H11" s="199"/>
-      <c r="I11" s="199"/>
-      <c r="J11" s="199"/>
-      <c r="K11" s="199"/>
-      <c r="L11" s="199"/>
-      <c r="M11" s="199"/>
-      <c r="N11" s="199"/>
+      <c r="B11" s="198"/>
+      <c r="C11" s="198"/>
+      <c r="D11" s="198"/>
+      <c r="E11" s="198"/>
+      <c r="F11" s="198"/>
+      <c r="G11" s="198"/>
+      <c r="H11" s="198"/>
+      <c r="I11" s="198"/>
+      <c r="J11" s="198"/>
+      <c r="K11" s="198"/>
+      <c r="L11" s="198"/>
+      <c r="M11" s="198"/>
+      <c r="N11" s="198"/>
       <c r="O11" s="36"/>
       <c r="P11" s="36"/>
     </row>
     <row r="12" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="24"/>
-      <c r="B12" s="206"/>
-      <c r="C12" s="206"/>
-      <c r="D12" s="206"/>
-      <c r="E12" s="206"/>
-      <c r="F12" s="206"/>
-      <c r="G12" s="206"/>
-      <c r="H12" s="206"/>
-      <c r="I12" s="206"/>
-      <c r="J12" s="206"/>
-      <c r="K12" s="206"/>
-      <c r="L12" s="206"/>
-      <c r="M12" s="206"/>
-      <c r="N12" s="206"/>
+      <c r="B12" s="205"/>
+      <c r="C12" s="205"/>
+      <c r="D12" s="205"/>
+      <c r="E12" s="205"/>
+      <c r="F12" s="205"/>
+      <c r="G12" s="205"/>
+      <c r="H12" s="205"/>
+      <c r="I12" s="205"/>
+      <c r="J12" s="205"/>
+      <c r="K12" s="205"/>
+      <c r="L12" s="205"/>
+      <c r="M12" s="205"/>
+      <c r="N12" s="205"/>
       <c r="O12" s="36"/>
       <c r="P12" s="36"/>
     </row>
@@ -5959,37 +5954,37 @@
       <c r="A13" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="199"/>
-      <c r="C13" s="199"/>
-      <c r="D13" s="199"/>
-      <c r="E13" s="199"/>
-      <c r="F13" s="199"/>
-      <c r="G13" s="199"/>
-      <c r="H13" s="199"/>
-      <c r="I13" s="199"/>
-      <c r="J13" s="199"/>
-      <c r="K13" s="199"/>
-      <c r="L13" s="199"/>
-      <c r="M13" s="199"/>
-      <c r="N13" s="199"/>
+      <c r="B13" s="198"/>
+      <c r="C13" s="198"/>
+      <c r="D13" s="198"/>
+      <c r="E13" s="198"/>
+      <c r="F13" s="198"/>
+      <c r="G13" s="198"/>
+      <c r="H13" s="198"/>
+      <c r="I13" s="198"/>
+      <c r="J13" s="198"/>
+      <c r="K13" s="198"/>
+      <c r="L13" s="198"/>
+      <c r="M13" s="198"/>
+      <c r="N13" s="198"/>
       <c r="O13" s="36"/>
       <c r="P13" s="71"/>
     </row>
     <row r="14" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="44"/>
-      <c r="B14" s="206"/>
-      <c r="C14" s="206"/>
-      <c r="D14" s="206"/>
-      <c r="E14" s="206"/>
-      <c r="F14" s="206"/>
-      <c r="G14" s="206"/>
-      <c r="H14" s="206"/>
-      <c r="I14" s="206"/>
-      <c r="J14" s="206"/>
-      <c r="K14" s="206"/>
-      <c r="L14" s="206"/>
-      <c r="M14" s="206"/>
-      <c r="N14" s="206"/>
+      <c r="B14" s="205"/>
+      <c r="C14" s="205"/>
+      <c r="D14" s="205"/>
+      <c r="E14" s="205"/>
+      <c r="F14" s="205"/>
+      <c r="G14" s="205"/>
+      <c r="H14" s="205"/>
+      <c r="I14" s="205"/>
+      <c r="J14" s="205"/>
+      <c r="K14" s="205"/>
+      <c r="L14" s="205"/>
+      <c r="M14" s="205"/>
+      <c r="N14" s="205"/>
       <c r="O14" s="36"/>
       <c r="P14" s="56"/>
     </row>
@@ -5997,37 +5992,37 @@
       <c r="A15" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="199"/>
-      <c r="C15" s="199"/>
-      <c r="D15" s="199"/>
-      <c r="E15" s="199"/>
-      <c r="F15" s="199"/>
-      <c r="G15" s="199"/>
-      <c r="H15" s="199"/>
-      <c r="I15" s="199"/>
-      <c r="J15" s="199"/>
-      <c r="K15" s="199"/>
-      <c r="L15" s="199"/>
-      <c r="M15" s="199"/>
-      <c r="N15" s="199"/>
+      <c r="B15" s="198"/>
+      <c r="C15" s="198"/>
+      <c r="D15" s="198"/>
+      <c r="E15" s="198"/>
+      <c r="F15" s="198"/>
+      <c r="G15" s="198"/>
+      <c r="H15" s="198"/>
+      <c r="I15" s="198"/>
+      <c r="J15" s="198"/>
+      <c r="K15" s="198"/>
+      <c r="L15" s="198"/>
+      <c r="M15" s="198"/>
+      <c r="N15" s="198"/>
       <c r="O15" s="36"/>
       <c r="P15" s="47"/>
     </row>
     <row r="16" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="44"/>
-      <c r="B16" s="207"/>
-      <c r="C16" s="207"/>
-      <c r="D16" s="207"/>
-      <c r="E16" s="207"/>
-      <c r="F16" s="207"/>
-      <c r="G16" s="207"/>
-      <c r="H16" s="207"/>
-      <c r="I16" s="207"/>
-      <c r="J16" s="207"/>
-      <c r="K16" s="207"/>
-      <c r="L16" s="207"/>
-      <c r="M16" s="207"/>
-      <c r="N16" s="207"/>
+      <c r="B16" s="206"/>
+      <c r="C16" s="206"/>
+      <c r="D16" s="206"/>
+      <c r="E16" s="206"/>
+      <c r="F16" s="206"/>
+      <c r="G16" s="206"/>
+      <c r="H16" s="206"/>
+      <c r="I16" s="206"/>
+      <c r="J16" s="206"/>
+      <c r="K16" s="206"/>
+      <c r="L16" s="206"/>
+      <c r="M16" s="206"/>
+      <c r="N16" s="206"/>
       <c r="O16" s="36"/>
       <c r="P16" s="56"/>
     </row>
@@ -6081,27 +6076,27 @@
     </row>
     <row r="19" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="58"/>
-      <c r="B19" s="208"/>
+      <c r="B19" s="207"/>
       <c r="C19" s="17"/>
-      <c r="D19" s="208"/>
+      <c r="D19" s="207"/>
       <c r="E19" s="17"/>
       <c r="F19" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="G19" s="193" t="s">
+      <c r="G19" s="192" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="192"/>
+      <c r="H19" s="191"/>
       <c r="I19" s="138"/>
-      <c r="J19" s="193"/>
-      <c r="K19" s="192" t="s">
+      <c r="J19" s="192"/>
+      <c r="K19" s="191" t="s">
         <v>29</v>
       </c>
       <c r="L19" s="138"/>
-      <c r="M19" s="193" t="s">
+      <c r="M19" s="192" t="s">
         <v>87</v>
       </c>
-      <c r="N19" s="192"/>
+      <c r="N19" s="191"/>
       <c r="O19" s="36"/>
     </row>
     <row r="20" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6136,23 +6131,23 @@
     </row>
     <row r="21" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="67"/>
-      <c r="B21" s="208"/>
+      <c r="B21" s="207"/>
       <c r="C21" s="17"/>
-      <c r="D21" s="208"/>
+      <c r="D21" s="207"/>
       <c r="E21" s="17"/>
-      <c r="F21" s="194" t="s">
+      <c r="F21" s="193" t="s">
         <v>102</v>
       </c>
       <c r="G21" s="131" t="s">
         <v>62</v>
       </c>
       <c r="H21" s="185"/>
-      <c r="I21" s="194"/>
+      <c r="I21" s="193"/>
       <c r="J21" s="131"/>
       <c r="K21" s="185" t="s">
         <v>29</v>
       </c>
-      <c r="L21" s="194"/>
+      <c r="L21" s="193"/>
       <c r="M21" s="131" t="s">
         <v>87</v>
       </c>
@@ -6196,16 +6191,16 @@
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
       <c r="E23" s="38"/>
-      <c r="F23" s="209" t="s">
+      <c r="F23" s="208" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="209"/>
-      <c r="H23" s="209"/>
-      <c r="I23" s="209" t="s">
+      <c r="G23" s="208"/>
+      <c r="H23" s="208"/>
+      <c r="I23" s="208" t="s">
         <v>108</v>
       </c>
-      <c r="J23" s="209"/>
-      <c r="K23" s="209"/>
+      <c r="J23" s="208"/>
+      <c r="K23" s="208"/>
       <c r="L23" s="130" t="s">
         <v>108</v>
       </c>
@@ -6225,11 +6220,11 @@
         <v>23</v>
       </c>
       <c r="E24" s="38"/>
-      <c r="F24" s="210" t="s">
+      <c r="F24" s="209" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="210"/>
-      <c r="H24" s="210"/>
+      <c r="G24" s="209"/>
+      <c r="H24" s="209"/>
       <c r="I24" s="175" t="s">
         <v>105</v>
       </c>
@@ -6252,11 +6247,11 @@
       </c>
       <c r="G25" s="177"/>
       <c r="H25" s="177"/>
-      <c r="I25" s="209" t="s">
+      <c r="I25" s="208" t="s">
         <v>108</v>
       </c>
-      <c r="J25" s="209"/>
-      <c r="K25" s="209"/>
+      <c r="J25" s="208"/>
+      <c r="K25" s="208"/>
       <c r="L25" s="130" t="s">
         <v>108</v>
       </c>
@@ -6300,19 +6295,19 @@
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
       <c r="F27" s="138"/>
-      <c r="G27" s="193" t="s">
+      <c r="G27" s="192" t="s">
         <v>78</v>
       </c>
-      <c r="H27" s="192"/>
+      <c r="H27" s="191"/>
       <c r="I27" s="138" t="s">
         <v>78</v>
       </c>
-      <c r="J27" s="193"/>
-      <c r="K27" s="192"/>
+      <c r="J27" s="192"/>
+      <c r="K27" s="191"/>
       <c r="L27" s="138" t="s">
         <v>113</v>
       </c>
-      <c r="M27" s="193"/>
+      <c r="M27" s="192"/>
       <c r="N27" s="185" t="s">
         <v>78</v>
       </c>
@@ -6345,25 +6340,25 @@
     </row>
     <row r="29" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="74"/>
-      <c r="B29" s="211"/>
+      <c r="B29" s="210"/>
       <c r="C29" s="133"/>
-      <c r="D29" s="211"/>
+      <c r="D29" s="210"/>
       <c r="E29" s="133"/>
-      <c r="F29" s="212"/>
-      <c r="G29" s="213" t="s">
+      <c r="F29" s="211"/>
+      <c r="G29" s="212" t="s">
         <v>78</v>
       </c>
-      <c r="H29" s="214"/>
-      <c r="I29" s="212" t="s">
+      <c r="H29" s="213"/>
+      <c r="I29" s="211" t="s">
         <v>78</v>
       </c>
-      <c r="J29" s="213"/>
-      <c r="K29" s="214"/>
-      <c r="L29" s="212" t="s">
+      <c r="J29" s="212"/>
+      <c r="K29" s="213"/>
+      <c r="L29" s="211" t="s">
         <v>113</v>
       </c>
-      <c r="M29" s="213"/>
-      <c r="N29" s="214" t="s">
+      <c r="M29" s="212"/>
+      <c r="N29" s="213" t="s">
         <v>78</v>
       </c>
     </row>
@@ -6384,20 +6379,20 @@
       <c r="N30" s="80"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="215"/>
-      <c r="B31" s="216"/>
-      <c r="C31" s="216"/>
-      <c r="D31" s="216"/>
-      <c r="E31" s="216"/>
-      <c r="F31" s="216"/>
-      <c r="G31" s="216"/>
-      <c r="H31" s="216"/>
-      <c r="I31" s="216"/>
-      <c r="J31" s="216"/>
-      <c r="K31" s="216"/>
-      <c r="L31" s="216"/>
-      <c r="M31" s="216"/>
-      <c r="N31" s="216"/>
+      <c r="A31" s="214"/>
+      <c r="B31" s="215"/>
+      <c r="C31" s="215"/>
+      <c r="D31" s="215"/>
+      <c r="E31" s="215"/>
+      <c r="F31" s="215"/>
+      <c r="G31" s="215"/>
+      <c r="H31" s="215"/>
+      <c r="I31" s="215"/>
+      <c r="J31" s="215"/>
+      <c r="K31" s="215"/>
+      <c r="L31" s="215"/>
+      <c r="M31" s="215"/>
+      <c r="N31" s="215"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
@@ -6418,84 +6413,84 @@
       <c r="N32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="217" t="s">
+      <c r="A33" s="216" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="217"/>
-      <c r="C33" s="217"/>
-      <c r="D33" s="217"/>
-      <c r="E33" s="217"/>
-      <c r="F33" s="217"/>
-      <c r="G33" s="217"/>
-      <c r="H33" s="217"/>
-      <c r="I33" s="217"/>
-      <c r="J33" s="217"/>
-      <c r="K33" s="217"/>
-      <c r="L33" s="217"/>
-      <c r="M33" s="217"/>
-      <c r="N33" s="217"/>
-      <c r="O33" s="218"/>
+      <c r="B33" s="216"/>
+      <c r="C33" s="216"/>
+      <c r="D33" s="216"/>
+      <c r="E33" s="216"/>
+      <c r="F33" s="216"/>
+      <c r="G33" s="216"/>
+      <c r="H33" s="216"/>
+      <c r="I33" s="216"/>
+      <c r="J33" s="216"/>
+      <c r="K33" s="216"/>
+      <c r="L33" s="216"/>
+      <c r="M33" s="216"/>
+      <c r="N33" s="216"/>
+      <c r="O33" s="217"/>
     </row>
     <row r="34" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="219"/>
-      <c r="B34" s="220" t="s">
+      <c r="A34" s="218"/>
+      <c r="B34" s="219" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="220"/>
-      <c r="D34" s="221" t="s">
+      <c r="C34" s="219"/>
+      <c r="D34" s="220" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="221"/>
-      <c r="F34" s="222" t="s">
+      <c r="E34" s="220"/>
+      <c r="F34" s="221" t="s">
         <v>4</v>
       </c>
-      <c r="G34" s="222"/>
-      <c r="H34" s="222"/>
-      <c r="I34" s="221" t="s">
+      <c r="G34" s="221"/>
+      <c r="H34" s="221"/>
+      <c r="I34" s="220" t="s">
         <v>5</v>
       </c>
-      <c r="J34" s="221"/>
-      <c r="K34" s="221"/>
-      <c r="L34" s="220" t="s">
+      <c r="J34" s="220"/>
+      <c r="K34" s="220"/>
+      <c r="L34" s="219" t="s">
         <v>6</v>
       </c>
-      <c r="M34" s="220"/>
-      <c r="N34" s="220"/>
+      <c r="M34" s="219"/>
+      <c r="N34" s="219"/>
     </row>
     <row r="35" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="205"/>
-      <c r="C35" s="205"/>
-      <c r="D35" s="205"/>
-      <c r="E35" s="205"/>
-      <c r="F35" s="205"/>
-      <c r="G35" s="205"/>
-      <c r="H35" s="205"/>
-      <c r="I35" s="205"/>
-      <c r="J35" s="205"/>
-      <c r="K35" s="205"/>
-      <c r="L35" s="205"/>
-      <c r="M35" s="205"/>
-      <c r="N35" s="205"/>
+      <c r="B35" s="204"/>
+      <c r="C35" s="204"/>
+      <c r="D35" s="204"/>
+      <c r="E35" s="204"/>
+      <c r="F35" s="204"/>
+      <c r="G35" s="204"/>
+      <c r="H35" s="204"/>
+      <c r="I35" s="204"/>
+      <c r="J35" s="204"/>
+      <c r="K35" s="204"/>
+      <c r="L35" s="204"/>
+      <c r="M35" s="204"/>
+      <c r="N35" s="204"/>
       <c r="O35" s="91"/>
     </row>
     <row r="36" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="7"/>
-      <c r="B36" s="206"/>
-      <c r="C36" s="206"/>
-      <c r="D36" s="206"/>
-      <c r="E36" s="206"/>
-      <c r="F36" s="206"/>
-      <c r="G36" s="206"/>
-      <c r="H36" s="206"/>
-      <c r="I36" s="206"/>
-      <c r="J36" s="206"/>
-      <c r="K36" s="206"/>
-      <c r="L36" s="206"/>
-      <c r="M36" s="206"/>
-      <c r="N36" s="206"/>
+      <c r="B36" s="205"/>
+      <c r="C36" s="205"/>
+      <c r="D36" s="205"/>
+      <c r="E36" s="205"/>
+      <c r="F36" s="205"/>
+      <c r="G36" s="205"/>
+      <c r="H36" s="205"/>
+      <c r="I36" s="205"/>
+      <c r="J36" s="205"/>
+      <c r="K36" s="205"/>
+      <c r="L36" s="205"/>
+      <c r="M36" s="205"/>
+      <c r="N36" s="205"/>
       <c r="O36" s="91"/>
       <c r="P36" s="91"/>
     </row>
@@ -6503,36 +6498,36 @@
       <c r="A37" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="199"/>
-      <c r="C37" s="199"/>
-      <c r="D37" s="199"/>
-      <c r="E37" s="199"/>
-      <c r="F37" s="199"/>
-      <c r="G37" s="199"/>
-      <c r="H37" s="199"/>
-      <c r="I37" s="199"/>
-      <c r="J37" s="199"/>
-      <c r="K37" s="199"/>
-      <c r="L37" s="199"/>
-      <c r="M37" s="199"/>
-      <c r="N37" s="199"/>
+      <c r="B37" s="198"/>
+      <c r="C37" s="198"/>
+      <c r="D37" s="198"/>
+      <c r="E37" s="198"/>
+      <c r="F37" s="198"/>
+      <c r="G37" s="198"/>
+      <c r="H37" s="198"/>
+      <c r="I37" s="198"/>
+      <c r="J37" s="198"/>
+      <c r="K37" s="198"/>
+      <c r="L37" s="198"/>
+      <c r="M37" s="198"/>
+      <c r="N37" s="198"/>
       <c r="O37" s="34"/>
     </row>
     <row r="38" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="24"/>
-      <c r="B38" s="206"/>
-      <c r="C38" s="206"/>
-      <c r="D38" s="206"/>
-      <c r="E38" s="206"/>
-      <c r="F38" s="206"/>
-      <c r="G38" s="206"/>
-      <c r="H38" s="206"/>
-      <c r="I38" s="206"/>
-      <c r="J38" s="206"/>
-      <c r="K38" s="206"/>
-      <c r="L38" s="206"/>
-      <c r="M38" s="206"/>
-      <c r="N38" s="206"/>
+      <c r="B38" s="205"/>
+      <c r="C38" s="205"/>
+      <c r="D38" s="205"/>
+      <c r="E38" s="205"/>
+      <c r="F38" s="205"/>
+      <c r="G38" s="205"/>
+      <c r="H38" s="205"/>
+      <c r="I38" s="205"/>
+      <c r="J38" s="205"/>
+      <c r="K38" s="205"/>
+      <c r="L38" s="205"/>
+      <c r="M38" s="205"/>
+      <c r="N38" s="205"/>
       <c r="O38" s="36"/>
       <c r="P38" s="91"/>
     </row>
@@ -6540,37 +6535,37 @@
       <c r="A39" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="199"/>
-      <c r="C39" s="199"/>
-      <c r="D39" s="199"/>
-      <c r="E39" s="199"/>
-      <c r="F39" s="199"/>
-      <c r="G39" s="199"/>
-      <c r="H39" s="199"/>
-      <c r="I39" s="199"/>
-      <c r="J39" s="199"/>
-      <c r="K39" s="199"/>
-      <c r="L39" s="199"/>
-      <c r="M39" s="199"/>
-      <c r="N39" s="199"/>
+      <c r="B39" s="198"/>
+      <c r="C39" s="198"/>
+      <c r="D39" s="198"/>
+      <c r="E39" s="198"/>
+      <c r="F39" s="198"/>
+      <c r="G39" s="198"/>
+      <c r="H39" s="198"/>
+      <c r="I39" s="198"/>
+      <c r="J39" s="198"/>
+      <c r="K39" s="198"/>
+      <c r="L39" s="198"/>
+      <c r="M39" s="198"/>
+      <c r="N39" s="198"/>
       <c r="O39" s="36"/>
       <c r="P39" s="91"/>
     </row>
     <row r="40" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="24"/>
-      <c r="B40" s="206"/>
-      <c r="C40" s="206"/>
-      <c r="D40" s="206"/>
-      <c r="E40" s="206"/>
-      <c r="F40" s="206"/>
-      <c r="G40" s="206"/>
-      <c r="H40" s="206"/>
-      <c r="I40" s="206"/>
-      <c r="J40" s="206"/>
-      <c r="K40" s="206"/>
-      <c r="L40" s="206"/>
-      <c r="M40" s="206"/>
-      <c r="N40" s="206"/>
+      <c r="B40" s="205"/>
+      <c r="C40" s="205"/>
+      <c r="D40" s="205"/>
+      <c r="E40" s="205"/>
+      <c r="F40" s="205"/>
+      <c r="G40" s="205"/>
+      <c r="H40" s="205"/>
+      <c r="I40" s="205"/>
+      <c r="J40" s="205"/>
+      <c r="K40" s="205"/>
+      <c r="L40" s="205"/>
+      <c r="M40" s="205"/>
+      <c r="N40" s="205"/>
       <c r="O40" s="36"/>
       <c r="P40" s="91"/>
     </row>
@@ -6578,37 +6573,37 @@
       <c r="A41" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="199"/>
-      <c r="C41" s="199"/>
-      <c r="D41" s="199"/>
-      <c r="E41" s="199"/>
-      <c r="F41" s="199"/>
-      <c r="G41" s="199"/>
-      <c r="H41" s="199"/>
-      <c r="I41" s="199"/>
-      <c r="J41" s="199"/>
-      <c r="K41" s="199"/>
-      <c r="L41" s="199"/>
-      <c r="M41" s="199"/>
-      <c r="N41" s="199"/>
+      <c r="B41" s="198"/>
+      <c r="C41" s="198"/>
+      <c r="D41" s="198"/>
+      <c r="E41" s="198"/>
+      <c r="F41" s="198"/>
+      <c r="G41" s="198"/>
+      <c r="H41" s="198"/>
+      <c r="I41" s="198"/>
+      <c r="J41" s="198"/>
+      <c r="K41" s="198"/>
+      <c r="L41" s="198"/>
+      <c r="M41" s="198"/>
+      <c r="N41" s="198"/>
       <c r="O41" s="36"/>
       <c r="P41" s="91"/>
     </row>
     <row r="42" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="24"/>
-      <c r="B42" s="206"/>
-      <c r="C42" s="206"/>
-      <c r="D42" s="206"/>
-      <c r="E42" s="206"/>
-      <c r="F42" s="206"/>
-      <c r="G42" s="206"/>
-      <c r="H42" s="206"/>
-      <c r="I42" s="206"/>
-      <c r="J42" s="206"/>
-      <c r="K42" s="206"/>
-      <c r="L42" s="206"/>
-      <c r="M42" s="206"/>
-      <c r="N42" s="206"/>
+      <c r="B42" s="205"/>
+      <c r="C42" s="205"/>
+      <c r="D42" s="205"/>
+      <c r="E42" s="205"/>
+      <c r="F42" s="205"/>
+      <c r="G42" s="205"/>
+      <c r="H42" s="205"/>
+      <c r="I42" s="205"/>
+      <c r="J42" s="205"/>
+      <c r="K42" s="205"/>
+      <c r="L42" s="205"/>
+      <c r="M42" s="205"/>
+      <c r="N42" s="205"/>
       <c r="O42" s="91"/>
       <c r="P42" s="91"/>
     </row>
@@ -6616,37 +6611,37 @@
       <c r="A43" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="199"/>
-      <c r="C43" s="199"/>
-      <c r="D43" s="199"/>
-      <c r="E43" s="199"/>
-      <c r="F43" s="199"/>
-      <c r="G43" s="199"/>
-      <c r="H43" s="199"/>
-      <c r="I43" s="199"/>
-      <c r="J43" s="199"/>
-      <c r="K43" s="199"/>
-      <c r="L43" s="199"/>
-      <c r="M43" s="199"/>
-      <c r="N43" s="199"/>
+      <c r="B43" s="198"/>
+      <c r="C43" s="198"/>
+      <c r="D43" s="198"/>
+      <c r="E43" s="198"/>
+      <c r="F43" s="198"/>
+      <c r="G43" s="198"/>
+      <c r="H43" s="198"/>
+      <c r="I43" s="198"/>
+      <c r="J43" s="198"/>
+      <c r="K43" s="198"/>
+      <c r="L43" s="198"/>
+      <c r="M43" s="198"/>
+      <c r="N43" s="198"/>
       <c r="O43" s="91"/>
       <c r="P43" s="91"/>
     </row>
     <row r="44" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="44"/>
-      <c r="B44" s="206"/>
-      <c r="C44" s="206"/>
-      <c r="D44" s="206"/>
-      <c r="E44" s="206"/>
-      <c r="F44" s="206"/>
-      <c r="G44" s="206"/>
-      <c r="H44" s="206"/>
-      <c r="I44" s="206"/>
-      <c r="J44" s="206"/>
-      <c r="K44" s="206"/>
-      <c r="L44" s="206"/>
-      <c r="M44" s="206"/>
-      <c r="N44" s="206"/>
+      <c r="B44" s="205"/>
+      <c r="C44" s="205"/>
+      <c r="D44" s="205"/>
+      <c r="E44" s="205"/>
+      <c r="F44" s="205"/>
+      <c r="G44" s="205"/>
+      <c r="H44" s="205"/>
+      <c r="I44" s="205"/>
+      <c r="J44" s="205"/>
+      <c r="K44" s="205"/>
+      <c r="L44" s="205"/>
+      <c r="M44" s="205"/>
+      <c r="N44" s="205"/>
       <c r="O44" s="91"/>
       <c r="P44" s="91"/>
     </row>
@@ -6654,53 +6649,53 @@
       <c r="A45" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="199"/>
-      <c r="C45" s="199"/>
-      <c r="D45" s="199"/>
-      <c r="E45" s="199"/>
-      <c r="F45" s="199"/>
-      <c r="G45" s="199"/>
-      <c r="H45" s="199"/>
-      <c r="I45" s="199"/>
-      <c r="J45" s="199"/>
-      <c r="K45" s="199"/>
-      <c r="L45" s="199"/>
-      <c r="M45" s="199"/>
-      <c r="N45" s="199"/>
+      <c r="B45" s="198"/>
+      <c r="C45" s="198"/>
+      <c r="D45" s="198"/>
+      <c r="E45" s="198"/>
+      <c r="F45" s="198"/>
+      <c r="G45" s="198"/>
+      <c r="H45" s="198"/>
+      <c r="I45" s="198"/>
+      <c r="J45" s="198"/>
+      <c r="K45" s="198"/>
+      <c r="L45" s="198"/>
+      <c r="M45" s="198"/>
+      <c r="N45" s="198"/>
       <c r="O45" s="91"/>
     </row>
     <row r="46" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="44"/>
-      <c r="B46" s="207"/>
-      <c r="C46" s="207"/>
-      <c r="D46" s="207"/>
-      <c r="E46" s="207"/>
-      <c r="F46" s="207"/>
-      <c r="G46" s="207"/>
-      <c r="H46" s="207"/>
-      <c r="I46" s="207"/>
-      <c r="J46" s="207"/>
-      <c r="K46" s="207"/>
-      <c r="L46" s="207"/>
-      <c r="M46" s="207"/>
-      <c r="N46" s="207"/>
+      <c r="B46" s="206"/>
+      <c r="C46" s="206"/>
+      <c r="D46" s="206"/>
+      <c r="E46" s="206"/>
+      <c r="F46" s="206"/>
+      <c r="G46" s="206"/>
+      <c r="H46" s="206"/>
+      <c r="I46" s="206"/>
+      <c r="J46" s="206"/>
+      <c r="K46" s="206"/>
+      <c r="L46" s="206"/>
+      <c r="M46" s="206"/>
+      <c r="N46" s="206"/>
       <c r="O46" s="91"/>
     </row>
     <row r="47" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="223"/>
-      <c r="B47" s="223"/>
-      <c r="C47" s="223"/>
-      <c r="D47" s="223"/>
-      <c r="E47" s="223"/>
-      <c r="F47" s="223"/>
-      <c r="G47" s="223"/>
-      <c r="H47" s="223"/>
-      <c r="I47" s="223"/>
-      <c r="J47" s="223"/>
-      <c r="K47" s="223"/>
-      <c r="L47" s="223"/>
-      <c r="M47" s="223"/>
-      <c r="N47" s="223"/>
+      <c r="A47" s="222"/>
+      <c r="B47" s="222"/>
+      <c r="C47" s="222"/>
+      <c r="D47" s="222"/>
+      <c r="E47" s="222"/>
+      <c r="F47" s="222"/>
+      <c r="G47" s="222"/>
+      <c r="H47" s="222"/>
+      <c r="I47" s="222"/>
+      <c r="J47" s="222"/>
+      <c r="K47" s="222"/>
+      <c r="L47" s="222"/>
+      <c r="M47" s="222"/>
+      <c r="N47" s="222"/>
       <c r="O47" s="91"/>
     </row>
     <row r="48" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6711,21 +6706,21 @@
       <c r="C48" s="88"/>
       <c r="D48" s="87"/>
       <c r="E48" s="88"/>
-      <c r="F48" s="199" t="s">
+      <c r="F48" s="198" t="s">
         <v>114</v>
       </c>
-      <c r="G48" s="199"/>
-      <c r="H48" s="199"/>
-      <c r="I48" s="224" t="s">
+      <c r="G48" s="198"/>
+      <c r="H48" s="198"/>
+      <c r="I48" s="223" t="s">
         <v>115</v>
       </c>
-      <c r="J48" s="224"/>
-      <c r="K48" s="224"/>
-      <c r="L48" s="224" t="s">
+      <c r="J48" s="223"/>
+      <c r="K48" s="223"/>
+      <c r="L48" s="223" t="s">
         <v>116</v>
       </c>
-      <c r="M48" s="224"/>
-      <c r="N48" s="224"/>
+      <c r="M48" s="223"/>
+      <c r="N48" s="223"/>
       <c r="O48" s="91"/>
       <c r="P48" s="125" t="s">
         <v>117</v>
@@ -6734,15 +6729,15 @@
     </row>
     <row r="49" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="58"/>
-      <c r="B49" s="208"/>
+      <c r="B49" s="207"/>
       <c r="C49" s="17"/>
-      <c r="D49" s="208"/>
+      <c r="D49" s="207"/>
       <c r="E49" s="17"/>
-      <c r="F49" s="206" t="s">
+      <c r="F49" s="205" t="s">
         <v>29</v>
       </c>
-      <c r="G49" s="206"/>
-      <c r="H49" s="206"/>
+      <c r="G49" s="205"/>
+      <c r="H49" s="205"/>
       <c r="I49" s="130" t="s">
         <v>118</v>
       </c>
@@ -6763,11 +6758,11 @@
       <c r="C50" s="26"/>
       <c r="D50" s="27"/>
       <c r="E50" s="26"/>
-      <c r="F50" s="199" t="s">
+      <c r="F50" s="198" t="s">
         <v>114</v>
       </c>
-      <c r="G50" s="199"/>
-      <c r="H50" s="199"/>
+      <c r="G50" s="198"/>
+      <c r="H50" s="198"/>
       <c r="I50" s="129" t="s">
         <v>115</v>
       </c>
@@ -6785,15 +6780,15 @@
     </row>
     <row r="51" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="67"/>
-      <c r="B51" s="208"/>
+      <c r="B51" s="207"/>
       <c r="C51" s="17"/>
-      <c r="D51" s="208"/>
+      <c r="D51" s="207"/>
       <c r="E51" s="17"/>
-      <c r="F51" s="206" t="s">
+      <c r="F51" s="205" t="s">
         <v>29</v>
       </c>
-      <c r="G51" s="206"/>
-      <c r="H51" s="206"/>
+      <c r="G51" s="205"/>
+      <c r="H51" s="205"/>
       <c r="I51" s="130" t="s">
         <v>118</v>
       </c>
@@ -6823,13 +6818,13 @@
       </c>
       <c r="G52" s="129"/>
       <c r="H52" s="129"/>
-      <c r="I52" s="225" t="s">
+      <c r="I52" s="224" t="s">
         <v>121</v>
       </c>
-      <c r="J52" s="226" t="s">
+      <c r="J52" s="225" t="s">
         <v>122</v>
       </c>
-      <c r="K52" s="227" t="s">
+      <c r="K52" s="226" t="s">
         <v>123</v>
       </c>
       <c r="L52" s="129" t="s">
@@ -6853,10 +6848,10 @@
       </c>
       <c r="G53" s="130"/>
       <c r="H53" s="130"/>
-      <c r="I53" s="228" t="s">
+      <c r="I53" s="227" t="s">
         <v>29</v>
       </c>
-      <c r="J53" s="229" t="s">
+      <c r="J53" s="228" t="s">
         <v>126</v>
       </c>
       <c r="K53" s="164" t="s">
@@ -6882,18 +6877,18 @@
         <v>23</v>
       </c>
       <c r="E54" s="38"/>
-      <c r="F54" s="199" t="s">
+      <c r="F54" s="198" t="s">
         <v>127</v>
       </c>
-      <c r="G54" s="199"/>
-      <c r="H54" s="199"/>
-      <c r="I54" s="225" t="s">
+      <c r="G54" s="198"/>
+      <c r="H54" s="198"/>
+      <c r="I54" s="224" t="s">
         <v>121</v>
       </c>
-      <c r="J54" s="226" t="s">
+      <c r="J54" s="225" t="s">
         <v>122</v>
       </c>
-      <c r="K54" s="227" t="s">
+      <c r="K54" s="226" t="s">
         <v>123</v>
       </c>
       <c r="L54" s="129" t="s">
@@ -6912,15 +6907,15 @@
       <c r="C55" s="38"/>
       <c r="D55" s="38"/>
       <c r="E55" s="38"/>
-      <c r="F55" s="206" t="s">
+      <c r="F55" s="205" t="s">
         <v>12</v>
       </c>
-      <c r="G55" s="206"/>
-      <c r="H55" s="206"/>
-      <c r="I55" s="228" t="s">
+      <c r="G55" s="205"/>
+      <c r="H55" s="205"/>
+      <c r="I55" s="227" t="s">
         <v>29</v>
       </c>
-      <c r="J55" s="229" t="s">
+      <c r="J55" s="228" t="s">
         <v>126</v>
       </c>
       <c r="K55" s="164" t="s">
@@ -6946,24 +6941,24 @@
         <v>32</v>
       </c>
       <c r="E56" s="38"/>
-      <c r="F56" s="199" t="s">
+      <c r="F56" s="198" t="s">
         <v>127</v>
       </c>
-      <c r="G56" s="199"/>
-      <c r="H56" s="199"/>
-      <c r="I56" s="225" t="s">
+      <c r="G56" s="198"/>
+      <c r="H56" s="198"/>
+      <c r="I56" s="224" t="s">
         <v>129</v>
       </c>
-      <c r="J56" s="226" t="s">
+      <c r="J56" s="225" t="s">
         <v>130</v>
       </c>
-      <c r="K56" s="227" t="s">
+      <c r="K56" s="226" t="s">
         <v>131</v>
       </c>
-      <c r="L56" s="225" t="s">
+      <c r="L56" s="224" t="s">
         <v>114</v>
       </c>
-      <c r="M56" s="226" t="s">
+      <c r="M56" s="225" t="s">
         <v>132</v>
       </c>
       <c r="N56" s="169" t="s">
@@ -6978,27 +6973,27 @@
       <c r="C57" s="38"/>
       <c r="D57" s="38"/>
       <c r="E57" s="38"/>
-      <c r="F57" s="206" t="s">
+      <c r="F57" s="205" t="s">
         <v>12</v>
       </c>
-      <c r="G57" s="206"/>
-      <c r="H57" s="206"/>
-      <c r="I57" s="228" t="s">
+      <c r="G57" s="205"/>
+      <c r="H57" s="205"/>
+      <c r="I57" s="227" t="s">
         <v>39</v>
       </c>
-      <c r="J57" s="229" t="s">
+      <c r="J57" s="228" t="s">
         <v>90</v>
       </c>
       <c r="K57" s="164" t="s">
         <v>113</v>
       </c>
-      <c r="L57" s="228" t="s">
+      <c r="L57" s="227" t="s">
         <v>29</v>
       </c>
-      <c r="M57" s="229" t="s">
+      <c r="M57" s="228" t="s">
         <v>113</v>
       </c>
-      <c r="N57" s="230" t="s">
+      <c r="N57" s="229" t="s">
         <v>39</v>
       </c>
       <c r="O57" s="1"/>
@@ -7012,20 +7007,20 @@
       <c r="C58" s="26"/>
       <c r="D58" s="27"/>
       <c r="E58" s="26"/>
-      <c r="F58" s="225"/>
-      <c r="G58" s="231"/>
+      <c r="F58" s="224"/>
+      <c r="G58" s="230"/>
       <c r="H58" s="179"/>
-      <c r="I58" s="225" t="s">
+      <c r="I58" s="224" t="s">
         <v>129</v>
       </c>
-      <c r="J58" s="226" t="s">
+      <c r="J58" s="225" t="s">
         <v>130</v>
       </c>
-      <c r="K58" s="227" t="s">
+      <c r="K58" s="226" t="s">
         <v>131</v>
       </c>
-      <c r="L58" s="225"/>
-      <c r="M58" s="226" t="s">
+      <c r="L58" s="224"/>
+      <c r="M58" s="225" t="s">
         <v>132</v>
       </c>
       <c r="N58" s="169" t="s">
@@ -7036,27 +7031,27 @@
     </row>
     <row r="59" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="74"/>
-      <c r="B59" s="211"/>
+      <c r="B59" s="210"/>
       <c r="C59" s="133"/>
-      <c r="D59" s="211"/>
+      <c r="D59" s="210"/>
       <c r="E59" s="133"/>
-      <c r="F59" s="232"/>
-      <c r="G59" s="233"/>
-      <c r="H59" s="234"/>
-      <c r="I59" s="235" t="s">
+      <c r="F59" s="231"/>
+      <c r="G59" s="232"/>
+      <c r="H59" s="233"/>
+      <c r="I59" s="234" t="s">
         <v>39</v>
       </c>
-      <c r="J59" s="236" t="s">
+      <c r="J59" s="235" t="s">
         <v>90</v>
       </c>
-      <c r="K59" s="237" t="s">
+      <c r="K59" s="236" t="s">
         <v>113</v>
       </c>
-      <c r="L59" s="235"/>
-      <c r="M59" s="236" t="s">
+      <c r="L59" s="234"/>
+      <c r="M59" s="235" t="s">
         <v>113</v>
       </c>
-      <c r="N59" s="238" t="s">
+      <c r="N59" s="237" t="s">
         <v>39</v>
       </c>
       <c r="O59" s="1"/>
@@ -7431,8 +7426,8 @@
     <mergeCell ref="A58:A59"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="55" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="55" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7447,7 +7442,7 @@
   </sheetPr>
   <dimension ref="A2:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -7519,14 +7514,14 @@
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="239" t="s">
+      <c r="B5" s="238" t="s">
         <v>135</v>
       </c>
       <c r="C5" s="111"/>
-      <c r="D5" s="239"/>
+      <c r="D5" s="238"/>
       <c r="E5" s="111"/>
-      <c r="F5" s="199"/>
-      <c r="G5" s="199"/>
+      <c r="F5" s="198"/>
+      <c r="G5" s="198"/>
       <c r="H5" s="87"/>
       <c r="I5" s="88"/>
       <c r="J5" s="87"/>
@@ -7538,17 +7533,17 @@
     </row>
     <row r="6" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
-      <c r="B6" s="240" t="s">
+      <c r="B6" s="239" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="241"/>
-      <c r="D6" s="240"/>
-      <c r="E6" s="241"/>
-      <c r="F6" s="242"/>
-      <c r="G6" s="242"/>
-      <c r="H6" s="208"/>
+      <c r="C6" s="240"/>
+      <c r="D6" s="239"/>
+      <c r="E6" s="240"/>
+      <c r="F6" s="241"/>
+      <c r="G6" s="241"/>
+      <c r="H6" s="207"/>
       <c r="I6" s="17"/>
-      <c r="J6" s="208"/>
+      <c r="J6" s="207"/>
       <c r="K6" s="17"/>
       <c r="L6" s="186"/>
     </row>
@@ -7556,57 +7551,57 @@
       <c r="A7" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="239" t="s">
+      <c r="B7" s="238" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="243" t="s">
+      <c r="C7" s="242" t="s">
         <v>137</v>
       </c>
-      <c r="D7" s="239"/>
-      <c r="E7" s="243" t="s">
+      <c r="D7" s="238"/>
+      <c r="E7" s="242" t="s">
         <v>138</v>
       </c>
-      <c r="F7" s="199" t="s">
+      <c r="F7" s="198" t="s">
         <v>139</v>
       </c>
-      <c r="G7" s="199"/>
+      <c r="G7" s="198"/>
       <c r="H7" s="27"/>
       <c r="I7" s="26"/>
       <c r="J7" s="27"/>
       <c r="K7" s="26"/>
-      <c r="L7" s="244"/>
+      <c r="L7" s="243"/>
       <c r="M7" s="128" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="24"/>
-      <c r="B8" s="240" t="s">
+      <c r="B8" s="239" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="245" t="s">
+      <c r="C8" s="244" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="240"/>
-      <c r="E8" s="245" t="s">
+      <c r="D8" s="239"/>
+      <c r="E8" s="244" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="242" t="s">
+      <c r="F8" s="241" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="242"/>
-      <c r="H8" s="208"/>
+      <c r="G8" s="241"/>
+      <c r="H8" s="207"/>
       <c r="I8" s="17"/>
-      <c r="J8" s="208"/>
+      <c r="J8" s="207"/>
       <c r="K8" s="17"/>
-      <c r="L8" s="246"/>
+      <c r="L8" s="245"/>
       <c r="M8" s="36"/>
     </row>
     <row r="9" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="247" t="s">
+      <c r="B9" s="246" t="s">
         <v>135</v>
       </c>
       <c r="C9" s="32" t="s">
@@ -7616,10 +7611,10 @@
         <v>141</v>
       </c>
       <c r="E9" s="129"/>
-      <c r="F9" s="199" t="s">
+      <c r="F9" s="198" t="s">
         <v>139</v>
       </c>
-      <c r="G9" s="199"/>
+      <c r="G9" s="198"/>
       <c r="H9" s="38" t="s">
         <v>20</v>
       </c>
@@ -7628,52 +7623,52 @@
         <v>20</v>
       </c>
       <c r="K9" s="38"/>
-      <c r="L9" s="246"/>
+      <c r="L9" s="245"/>
       <c r="M9" s="70" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="24"/>
-      <c r="B10" s="248" t="s">
+      <c r="B10" s="247" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="249" t="s">
+      <c r="C10" s="248" t="s">
         <v>113</v>
       </c>
       <c r="D10" s="130" t="s">
         <v>143</v>
       </c>
       <c r="E10" s="130"/>
-      <c r="F10" s="206" t="s">
+      <c r="F10" s="205" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="206"/>
+      <c r="G10" s="205"/>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
       <c r="K10" s="38"/>
-      <c r="L10" s="246"/>
+      <c r="L10" s="245"/>
       <c r="M10" s="36"/>
     </row>
     <row r="11" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="250" t="s">
+      <c r="B11" s="249" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="250"/>
-      <c r="D11" s="239" t="s">
+      <c r="C11" s="249"/>
+      <c r="D11" s="238" t="s">
         <v>145</v>
       </c>
-      <c r="E11" s="243" t="s">
+      <c r="E11" s="242" t="s">
         <v>138</v>
       </c>
-      <c r="F11" s="251" t="s">
+      <c r="F11" s="250" t="s">
         <v>146</v>
       </c>
-      <c r="G11" s="251"/>
+      <c r="G11" s="250"/>
       <c r="H11" s="38" t="s">
         <v>23</v>
       </c>
@@ -7682,7 +7677,7 @@
         <v>23</v>
       </c>
       <c r="K11" s="38"/>
-      <c r="L11" s="246"/>
+      <c r="L11" s="245"/>
       <c r="M11" s="36"/>
     </row>
     <row r="12" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7691,10 +7686,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="130"/>
-      <c r="D12" s="240" t="s">
+      <c r="D12" s="239" t="s">
         <v>113</v>
       </c>
-      <c r="E12" s="245" t="s">
+      <c r="E12" s="244" t="s">
         <v>29</v>
       </c>
       <c r="F12" s="41" t="s">
@@ -7709,7 +7704,7 @@
         <v>32</v>
       </c>
       <c r="K12" s="38"/>
-      <c r="L12" s="246"/>
+      <c r="L12" s="245"/>
     </row>
     <row r="13" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="44" t="s">
@@ -7719,21 +7714,21 @@
         <v>144</v>
       </c>
       <c r="C13" s="129"/>
-      <c r="D13" s="247" t="s">
+      <c r="D13" s="246" t="s">
         <v>145</v>
       </c>
       <c r="E13" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="F13" s="251" t="s">
+      <c r="F13" s="250" t="s">
         <v>146</v>
       </c>
-      <c r="G13" s="251"/>
+      <c r="G13" s="250"/>
       <c r="H13" s="38"/>
       <c r="I13" s="38"/>
       <c r="J13" s="38"/>
       <c r="K13" s="38"/>
-      <c r="L13" s="246"/>
+      <c r="L13" s="245"/>
     </row>
     <row r="14" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="44"/>
@@ -7741,10 +7736,10 @@
         <v>14</v>
       </c>
       <c r="C14" s="130"/>
-      <c r="D14" s="248" t="s">
+      <c r="D14" s="247" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="249" t="s">
+      <c r="E14" s="248" t="s">
         <v>29</v>
       </c>
       <c r="F14" s="41" t="s">
@@ -7755,170 +7750,170 @@
       <c r="I14" s="38"/>
       <c r="J14" s="38"/>
       <c r="K14" s="38"/>
-      <c r="L14" s="246"/>
+      <c r="L14" s="245"/>
     </row>
     <row r="15" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="252"/>
-      <c r="C15" s="253"/>
-      <c r="D15" s="252"/>
-      <c r="E15" s="253"/>
-      <c r="F15" s="252"/>
-      <c r="G15" s="253"/>
+      <c r="B15" s="251"/>
+      <c r="C15" s="252"/>
+      <c r="D15" s="251"/>
+      <c r="E15" s="252"/>
+      <c r="F15" s="251"/>
+      <c r="G15" s="252"/>
       <c r="H15" s="38"/>
       <c r="I15" s="38"/>
       <c r="J15" s="38"/>
       <c r="K15" s="38"/>
-      <c r="L15" s="246"/>
+      <c r="L15" s="245"/>
     </row>
     <row r="16" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="44"/>
       <c r="B16" s="152"/>
-      <c r="C16" s="234"/>
+      <c r="C16" s="233"/>
       <c r="D16" s="152"/>
-      <c r="E16" s="234"/>
+      <c r="E16" s="233"/>
       <c r="F16" s="152"/>
-      <c r="G16" s="234"/>
-      <c r="H16" s="254"/>
+      <c r="G16" s="233"/>
+      <c r="H16" s="253"/>
       <c r="I16" s="133"/>
-      <c r="J16" s="254"/>
+      <c r="J16" s="253"/>
       <c r="K16" s="133"/>
-      <c r="L16" s="246"/>
+      <c r="L16" s="245"/>
     </row>
     <row r="17" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="255"/>
-      <c r="B17" s="255"/>
-      <c r="C17" s="255"/>
-      <c r="D17" s="255"/>
-      <c r="E17" s="255"/>
-      <c r="F17" s="255"/>
-      <c r="G17" s="255"/>
-      <c r="H17" s="255"/>
-      <c r="I17" s="255"/>
-      <c r="J17" s="255"/>
-      <c r="K17" s="255"/>
-      <c r="L17" s="246"/>
+      <c r="A17" s="254"/>
+      <c r="B17" s="254"/>
+      <c r="C17" s="254"/>
+      <c r="D17" s="254"/>
+      <c r="E17" s="254"/>
+      <c r="F17" s="254"/>
+      <c r="G17" s="254"/>
+      <c r="H17" s="254"/>
+      <c r="I17" s="254"/>
+      <c r="J17" s="254"/>
+      <c r="K17" s="254"/>
+      <c r="L17" s="245"/>
     </row>
     <row r="18" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="256"/>
-      <c r="C18" s="257"/>
-      <c r="D18" s="256"/>
-      <c r="E18" s="257"/>
-      <c r="F18" s="256"/>
-      <c r="G18" s="257"/>
-      <c r="H18" s="256"/>
-      <c r="I18" s="257"/>
-      <c r="J18" s="256"/>
-      <c r="K18" s="257"/>
-      <c r="L18" s="246"/>
+      <c r="B18" s="255"/>
+      <c r="C18" s="256"/>
+      <c r="D18" s="255"/>
+      <c r="E18" s="256"/>
+      <c r="F18" s="255"/>
+      <c r="G18" s="256"/>
+      <c r="H18" s="255"/>
+      <c r="I18" s="256"/>
+      <c r="J18" s="255"/>
+      <c r="K18" s="256"/>
+      <c r="L18" s="245"/>
     </row>
     <row r="19" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="58"/>
-      <c r="B19" s="258"/>
-      <c r="C19" s="259"/>
-      <c r="D19" s="258"/>
-      <c r="E19" s="259"/>
-      <c r="F19" s="258"/>
-      <c r="G19" s="259"/>
-      <c r="H19" s="258"/>
-      <c r="I19" s="259"/>
-      <c r="J19" s="258"/>
-      <c r="K19" s="259"/>
-      <c r="L19" s="246"/>
+      <c r="B19" s="257"/>
+      <c r="C19" s="258"/>
+      <c r="D19" s="257"/>
+      <c r="E19" s="258"/>
+      <c r="F19" s="257"/>
+      <c r="G19" s="258"/>
+      <c r="H19" s="257"/>
+      <c r="I19" s="258"/>
+      <c r="J19" s="257"/>
+      <c r="K19" s="258"/>
+      <c r="L19" s="245"/>
     </row>
     <row r="20" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="231"/>
+      <c r="B20" s="230"/>
       <c r="C20" s="179"/>
-      <c r="D20" s="231"/>
+      <c r="D20" s="230"/>
       <c r="E20" s="179"/>
-      <c r="F20" s="231"/>
+      <c r="F20" s="230"/>
       <c r="G20" s="179"/>
-      <c r="H20" s="231"/>
+      <c r="H20" s="230"/>
       <c r="I20" s="179"/>
-      <c r="J20" s="231"/>
+      <c r="J20" s="230"/>
       <c r="K20" s="179"/>
-      <c r="L20" s="246"/>
+      <c r="L20" s="245"/>
     </row>
     <row r="21" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="67"/>
-      <c r="B21" s="260"/>
-      <c r="C21" s="259"/>
-      <c r="D21" s="260"/>
-      <c r="E21" s="259"/>
-      <c r="F21" s="260"/>
-      <c r="G21" s="259"/>
-      <c r="H21" s="260"/>
-      <c r="I21" s="259"/>
-      <c r="J21" s="260"/>
-      <c r="K21" s="259"/>
-      <c r="L21" s="246"/>
+      <c r="B21" s="259"/>
+      <c r="C21" s="258"/>
+      <c r="D21" s="259"/>
+      <c r="E21" s="258"/>
+      <c r="F21" s="259"/>
+      <c r="G21" s="258"/>
+      <c r="H21" s="259"/>
+      <c r="I21" s="258"/>
+      <c r="J21" s="259"/>
+      <c r="K21" s="258"/>
+      <c r="L21" s="245"/>
     </row>
     <row r="22" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="67" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="172"/>
-      <c r="C22" s="261"/>
+      <c r="C22" s="260"/>
       <c r="D22" s="172"/>
-      <c r="E22" s="261"/>
+      <c r="E22" s="260"/>
       <c r="F22" s="172"/>
-      <c r="G22" s="261"/>
+      <c r="G22" s="260"/>
       <c r="H22" s="172"/>
-      <c r="I22" s="261"/>
+      <c r="I22" s="260"/>
       <c r="J22" s="172"/>
-      <c r="K22" s="261"/>
+      <c r="K22" s="260"/>
       <c r="L22" s="186"/>
     </row>
     <row r="23" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="67"/>
       <c r="B23" s="170"/>
-      <c r="C23" s="262"/>
+      <c r="C23" s="261"/>
       <c r="D23" s="170"/>
-      <c r="E23" s="262"/>
+      <c r="E23" s="261"/>
       <c r="F23" s="170"/>
-      <c r="G23" s="262"/>
+      <c r="G23" s="261"/>
       <c r="H23" s="170"/>
-      <c r="I23" s="262"/>
+      <c r="I23" s="261"/>
       <c r="J23" s="170"/>
-      <c r="K23" s="262"/>
+      <c r="K23" s="261"/>
       <c r="L23" s="186"/>
     </row>
     <row r="24" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="263"/>
-      <c r="C24" s="261"/>
-      <c r="D24" s="263"/>
-      <c r="E24" s="261"/>
-      <c r="F24" s="263"/>
-      <c r="G24" s="261"/>
-      <c r="H24" s="263"/>
-      <c r="I24" s="261"/>
-      <c r="J24" s="263"/>
-      <c r="K24" s="261"/>
+      <c r="B24" s="262"/>
+      <c r="C24" s="260"/>
+      <c r="D24" s="262"/>
+      <c r="E24" s="260"/>
+      <c r="F24" s="262"/>
+      <c r="G24" s="260"/>
+      <c r="H24" s="262"/>
+      <c r="I24" s="260"/>
+      <c r="J24" s="262"/>
+      <c r="K24" s="260"/>
       <c r="L24" s="186"/>
     </row>
     <row r="25" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="67"/>
-      <c r="B25" s="264"/>
-      <c r="C25" s="262"/>
-      <c r="D25" s="264"/>
-      <c r="E25" s="262"/>
-      <c r="F25" s="264"/>
-      <c r="G25" s="262"/>
-      <c r="H25" s="264"/>
-      <c r="I25" s="262"/>
-      <c r="J25" s="264"/>
-      <c r="K25" s="262"/>
+      <c r="B25" s="263"/>
+      <c r="C25" s="261"/>
+      <c r="D25" s="263"/>
+      <c r="E25" s="261"/>
+      <c r="F25" s="263"/>
+      <c r="G25" s="261"/>
+      <c r="H25" s="263"/>
+      <c r="I25" s="261"/>
+      <c r="J25" s="263"/>
+      <c r="K25" s="261"/>
       <c r="L25" s="186"/>
     </row>
     <row r="26" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7969,16 +7964,16 @@
     </row>
     <row r="29" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="74"/>
-      <c r="B29" s="265"/>
-      <c r="C29" s="266"/>
-      <c r="D29" s="265"/>
-      <c r="E29" s="266"/>
-      <c r="F29" s="265"/>
-      <c r="G29" s="266"/>
-      <c r="H29" s="265"/>
-      <c r="I29" s="266"/>
-      <c r="J29" s="265"/>
-      <c r="K29" s="266"/>
+      <c r="B29" s="264"/>
+      <c r="C29" s="265"/>
+      <c r="D29" s="264"/>
+      <c r="E29" s="265"/>
+      <c r="F29" s="264"/>
+      <c r="G29" s="265"/>
+      <c r="H29" s="264"/>
+      <c r="I29" s="265"/>
+      <c r="J29" s="264"/>
+      <c r="K29" s="265"/>
       <c r="L29" s="186"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8185,8 +8180,8 @@
     <mergeCell ref="A28:A29"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="55" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="55" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>